<commit_message>
Fixed some issues with excel report
</commit_message>
<xml_diff>
--- a/org.pklose.espl/org.pklose.espl.tests/myReport.xlsx
+++ b/org.pklose.espl/org.pklose.espl.tests/myReport.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>Expected BRE Name</t>
   </si>
@@ -31,6 +31,18 @@
   </si>
   <si>
     <t>Actual BRE Type</t>
+  </si>
+  <si>
+    <t>PersonToPerson</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -101,6 +113,28 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="true"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -135,6 +169,28 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="true"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>